<commit_message>
after running cases A-F for the first time
</commit_message>
<xml_diff>
--- a/results/A-01.xlsx
+++ b/results/A-01.xlsx
@@ -733,37 +733,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-6488.624785711965</v>
+        <v>-6472.5345434786</v>
       </c>
       <c r="C2">
-        <v>13594.02038800302</v>
+        <v>13561.10628116392</v>
       </c>
       <c r="D2">
-        <v>-6488.624801366023</v>
+        <v>-6472.534545050638</v>
       </c>
       <c r="E2">
-        <v>-616.7708009249136</v>
+        <v>-616.0371926347913</v>
       </c>
       <c r="F2">
-        <v>56.11058059683239</v>
+        <v>55.96194096546753</v>
       </c>
       <c r="G2">
-        <v>45.57713514968538</v>
+        <v>45.63458162350963</v>
       </c>
       <c r="H2">
-        <v>56.39562259573745</v>
+        <v>56.24114139383937</v>
       </c>
       <c r="I2">
-        <v>45.36155323300659</v>
+        <v>45.42231789641141</v>
       </c>
       <c r="J2">
-        <v>56.11058059784779</v>
+        <v>55.9619409655719</v>
       </c>
       <c r="K2">
-        <v>45.5771351629333</v>
+        <v>45.63458162497881</v>
       </c>
       <c r="L2">
-        <v>54.26946397958852</v>
+        <v>54.24647791925514</v>
       </c>
       <c r="M2">
         <v>45</v>
@@ -772,22 +772,22 @@
         <v>65</v>
       </c>
       <c r="O2">
-        <v>45.5799708742814</v>
+        <v>45.62699102690868</v>
       </c>
       <c r="P2">
-        <v>54.26946400195146</v>
+        <v>54.24647792150091</v>
       </c>
       <c r="Q2">
         <v>45</v>
       </c>
       <c r="R2">
-        <v>8.800030366226681</v>
+        <v>8.953380639800754</v>
       </c>
       <c r="S2">
-        <v>-17.60006076390322</v>
+        <v>-17.90676128295929</v>
       </c>
       <c r="T2">
-        <v>8.80003039767654</v>
+        <v>8.953380643158548</v>
       </c>
       <c r="U2">
         <v>10</v>
@@ -799,13 +799,13 @@
         <v>10</v>
       </c>
       <c r="X2">
-        <v>-90.20640322799842</v>
+        <v>-92.33646748703023</v>
       </c>
       <c r="Y2">
-        <v>-144.5430218416236</v>
+        <v>-142.3360080380841</v>
       </c>
       <c r="Z2">
-        <v>-90.20640322799838</v>
+        <v>-92.33646748703015</v>
       </c>
       <c r="AB2">
         <v>10</v>
@@ -817,91 +817,91 @@
         <v>10</v>
       </c>
       <c r="AE2">
-        <v>-8.800030366226681</v>
+        <v>-8.953380639800754</v>
       </c>
       <c r="AF2">
-        <v>8.80003039767654</v>
+        <v>8.953380643158548</v>
       </c>
       <c r="AG2">
-        <v>8.800030366226681</v>
+        <v>8.953380639800754</v>
       </c>
       <c r="AH2">
-        <v>-17.60006076390322</v>
+        <v>-17.90676128295929</v>
       </c>
       <c r="AI2">
-        <v>8.80003039767654</v>
+        <v>8.953380643158548</v>
       </c>
       <c r="AJ2">
-        <v>8.800030366226681</v>
+        <v>8.953380639800754</v>
       </c>
       <c r="AK2">
-        <v>-8.80003039767654</v>
+        <v>-8.953380643158548</v>
       </c>
       <c r="AL2">
-        <v>27.16830930681258</v>
+        <v>24.99977027552693</v>
       </c>
       <c r="AM2">
-        <v>-27.16830930681257</v>
+        <v>-24.99977027552692</v>
       </c>
       <c r="AN2">
-        <v>-90.20640322799842</v>
+        <v>-92.33646748703023</v>
       </c>
       <c r="AO2">
-        <v>-144.5430218416236</v>
+        <v>-142.3360080380841</v>
       </c>
       <c r="AP2">
-        <v>-90.20640322799838</v>
+        <v>-92.33646748703015</v>
       </c>
       <c r="AQ2">
-        <v>-27.16830930681258</v>
+        <v>-24.99977027552693</v>
       </c>
       <c r="AR2">
-        <v>27.16830930681257</v>
+        <v>24.99977027552692</v>
       </c>
       <c r="AS2">
-        <v>56.11058059683239</v>
+        <v>55.96194096546753</v>
       </c>
       <c r="AT2">
-        <v>56.11058059683239</v>
+        <v>55.96194096546753</v>
       </c>
       <c r="AU2">
-        <v>56.39562259573739</v>
+        <v>56.24114139383931</v>
       </c>
       <c r="AV2">
-        <v>56.39562259573739</v>
+        <v>56.24114139383931</v>
       </c>
       <c r="AW2">
-        <v>56.39562259573745</v>
+        <v>56.24114139383937</v>
       </c>
       <c r="AX2">
-        <v>56.11058059784779</v>
+        <v>55.9619409655719</v>
       </c>
       <c r="AY2">
-        <v>56.11058059784779</v>
+        <v>55.9619409655719</v>
       </c>
       <c r="AZ2">
-        <v>45.57713514968538</v>
+        <v>45.63458162350963</v>
       </c>
       <c r="BA2">
-        <v>45.57713514968538</v>
+        <v>45.63458162350963</v>
       </c>
       <c r="BB2">
-        <v>45.36155323300659</v>
+        <v>45.42231789641141</v>
       </c>
       <c r="BC2">
-        <v>45.36155322604117</v>
+        <v>45.4223178956417</v>
       </c>
       <c r="BD2">
-        <v>45.36155323997207</v>
+        <v>45.4223178971809</v>
       </c>
       <c r="BE2">
-        <v>45.5771351629333</v>
+        <v>45.63458162497881</v>
       </c>
       <c r="BF2">
-        <v>45.57713516293336</v>
+        <v>45.63458162497881</v>
       </c>
       <c r="BG2">
-        <v>54.26946397958852</v>
+        <v>54.24647791925514</v>
       </c>
       <c r="BH2">
         <v>45</v>
@@ -910,10 +910,10 @@
         <v>65</v>
       </c>
       <c r="BJ2">
-        <v>45.5799708742814</v>
+        <v>45.62699102690868</v>
       </c>
       <c r="BK2">
-        <v>54.26946400195146</v>
+        <v>54.24647792150091</v>
       </c>
       <c r="BL2">
         <v>45</v>

</xml_diff>